<commit_message>
adding modified signupdata file
</commit_message>
<xml_diff>
--- a/src/test/java/com/ems/testdata/SignUpData.xlsx
+++ b/src/test/java/com/ems/testdata/SignUpData.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8CDF0D7-AF75-4C6C-A4DE-FF408586B683}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="8475" windowWidth="22890" xWindow="0" yWindow="2520"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
   <si>
     <t>First_Name</t>
   </si>
@@ -59,17 +59,13 @@
   </si>
   <si>
     <t>Abcd@1237</t>
-  </si>
-  <si>
-    <t>failed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,22 +136,22 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -172,10 +168,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -373,21 +369,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -404,7 +400,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -456,31 +452,31 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="27.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="25.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="22.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="1" max="1" width="27" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" ht="23.25" r="1" s="3" spans="1:6">
+    <row r="1" spans="1:6" s="3" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -500,7 +496,7 @@
         <v>5</v>
       </c>
     </row>
-    <row ht="23.25" r="2" spans="1:6">
+    <row r="2" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -519,11 +515,8 @@
       <c r="F2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row ht="23.25" r="3" spans="1:6">
+    <row r="3" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -542,11 +535,8 @@
       <c r="F3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H3" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row ht="23.25" r="4" spans="1:6">
+    <row r="4" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -565,11 +555,8 @@
       <c r="F4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H4" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row ht="23.25" r="5" spans="1:6">
+    <row r="5" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -588,12 +575,9 @@
       <c r="F5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H5" t="s">
-        <v>13</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>